<commit_message>
Renaming Affiliere import/export class. Affiliere can now read both xlsx and json files.
</commit_message>
<xml_diff>
--- a/test/lerfob/carbonbalancetool/productionlines/affiliere/resultat_reconciled_mod.xlsx
+++ b/test/lerfob/carbonbalancetool/productionlines/affiliere/resultat_reconciled_mod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/mathieu_fortin_nrcan-rncan_gc_ca/Documents/Documents/7_Developpement/JavaProjects/CAT/test/lerfob/carbonbalancetool/productionlines/affiliere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{0B497484-7275-4C09-A856-A1934553FE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3AE14F9-89B0-4163-9D2D-3FBD8DDE511A}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{0B497484-7275-4C09-A856-A1934553FE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DBF2761-D8D8-489D-AC25-2B402D47066D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8790" windowWidth="29040" windowHeight="15720" tabRatio="704" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-10380" windowWidth="29040" windowHeight="15720" tabRatio="704" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etiquettes" sheetId="1" r:id="rId1"/>
@@ -1990,7 +1990,17 @@
     <xf numFmtId="0" fontId="33" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2000,19 +2010,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2026,68 +2088,9 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2114,9 +2117,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="13"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -2366,6 +2366,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2841,8 +2845,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="141" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="141" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="142" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="142" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.7265625" customWidth="1"/>
@@ -2853,12 +2857,12 @@
     <col min="14" max="14" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="141" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:15" s="142" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="141" customFormat="1">
+    <row r="2" spans="1:15" s="142" customFormat="1">
       <c r="A2" s="79" t="s">
         <v>134</v>
       </c>
@@ -2866,7 +2870,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="141" customFormat="1">
+    <row r="3" spans="1:15" s="142" customFormat="1">
       <c r="A3" s="80" t="s">
         <v>136</v>
       </c>
@@ -2874,7 +2878,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="141" customFormat="1">
+    <row r="4" spans="1:15" s="142" customFormat="1">
       <c r="A4" s="80" t="s">
         <v>138</v>
       </c>
@@ -2882,7 +2886,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="141" customFormat="1">
+    <row r="5" spans="1:15" s="142" customFormat="1">
       <c r="A5" s="80" t="s">
         <v>140</v>
       </c>
@@ -2890,7 +2894,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="141" customFormat="1">
+    <row r="6" spans="1:15" s="142" customFormat="1">
       <c r="A6" s="80" t="s">
         <v>141</v>
       </c>
@@ -2898,7 +2902,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="141" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+    <row r="7" spans="1:15" s="142" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A7" s="81" t="s">
         <v>143</v>
       </c>
@@ -2907,21 +2911,21 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="C8" s="139" t="s">
+      <c r="C8" s="140" t="s">
         <v>268</v>
       </c>
-      <c r="D8" s="140"/>
-      <c r="E8" s="140"/>
-      <c r="F8" s="140"/>
-      <c r="G8" s="140"/>
-      <c r="H8" s="140"/>
-      <c r="I8" s="140"/>
-      <c r="J8" s="140"/>
-      <c r="K8" s="140"/>
-      <c r="L8" s="140"/>
-      <c r="M8" s="140"/>
-      <c r="N8" s="140"/>
-      <c r="O8" s="140"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="141"/>
+      <c r="F8" s="141"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="141"/>
+      <c r="M8" s="141"/>
+      <c r="N8" s="141"/>
+      <c r="O8" s="141"/>
     </row>
     <row r="9" spans="1:15">
       <c r="C9" t="s">
@@ -3136,21 +3140,21 @@
       </c>
     </row>
     <row r="28" spans="3:15">
-      <c r="C28" s="139" t="s">
+      <c r="C28" s="140" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="140"/>
-      <c r="E28" s="140"/>
-      <c r="F28" s="140"/>
-      <c r="G28" s="140"/>
-      <c r="H28" s="140"/>
-      <c r="I28" s="140"/>
-      <c r="J28" s="140"/>
-      <c r="K28" s="140"/>
-      <c r="L28" s="140"/>
-      <c r="M28" s="140"/>
-      <c r="N28" s="140"/>
-      <c r="O28" s="140"/>
+      <c r="D28" s="141"/>
+      <c r="E28" s="141"/>
+      <c r="F28" s="141"/>
+      <c r="G28" s="141"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="141"/>
+      <c r="J28" s="141"/>
+      <c r="K28" s="141"/>
+      <c r="L28" s="141"/>
+      <c r="M28" s="141"/>
+      <c r="N28" s="141"/>
+      <c r="O28" s="141"/>
     </row>
     <row r="29" spans="3:15">
       <c r="C29" t="s">
@@ -3366,21 +3370,21 @@
       </c>
     </row>
     <row r="44" spans="3:15">
-      <c r="C44" s="139" t="s">
+      <c r="C44" s="140" t="s">
         <v>297</v>
       </c>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140"/>
-      <c r="H44" s="140"/>
-      <c r="I44" s="140"/>
-      <c r="J44" s="140"/>
-      <c r="K44" s="140"/>
-      <c r="L44" s="140"/>
-      <c r="M44" s="140"/>
-      <c r="N44" s="140"/>
-      <c r="O44" s="140"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="141"/>
+      <c r="F44" s="141"/>
+      <c r="G44" s="141"/>
+      <c r="H44" s="141"/>
+      <c r="I44" s="141"/>
+      <c r="J44" s="141"/>
+      <c r="K44" s="141"/>
+      <c r="L44" s="141"/>
+      <c r="M44" s="141"/>
+      <c r="N44" s="141"/>
+      <c r="O44" s="141"/>
     </row>
     <row r="45" spans="3:15">
       <c r="C45" t="s">
@@ -3466,8 +3470,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="142" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="142" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="143" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="143" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7265625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
@@ -3477,12 +3481,12 @@
     <col min="9" max="16384" width="11.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="142" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:9" s="143" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="142" customFormat="1">
+    <row r="2" spans="1:9" s="143" customFormat="1">
       <c r="A2" s="79" t="s">
         <v>134</v>
       </c>
@@ -3490,7 +3494,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="142" customFormat="1">
+    <row r="3" spans="1:9" s="143" customFormat="1">
       <c r="A3" s="80" t="s">
         <v>136</v>
       </c>
@@ -3498,7 +3502,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="142" customFormat="1">
+    <row r="4" spans="1:9" s="143" customFormat="1">
       <c r="A4" s="80" t="s">
         <v>138</v>
       </c>
@@ -3506,7 +3510,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="142" customFormat="1">
+    <row r="5" spans="1:9" s="143" customFormat="1">
       <c r="A5" s="80" t="s">
         <v>140</v>
       </c>
@@ -3514,7 +3518,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="142" customFormat="1">
+    <row r="6" spans="1:9" s="143" customFormat="1">
       <c r="A6" s="80" t="s">
         <v>141</v>
       </c>
@@ -3522,7 +3526,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="142" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+    <row r="7" spans="1:9" s="143" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A7" s="81" t="s">
         <v>143</v>
       </c>
@@ -3531,10 +3535,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1">
-      <c r="C8" s="143" t="s">
+      <c r="C8" s="144" t="s">
         <v>307</v>
       </c>
-      <c r="D8" s="144"/>
+      <c r="D8" s="145"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
@@ -3899,20 +3903,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="141" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="141" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="142" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="142" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7265625" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="141" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:5" s="142" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="141" customFormat="1">
+    <row r="2" spans="1:5" s="142" customFormat="1">
       <c r="A2" s="79" t="s">
         <v>134</v>
       </c>
@@ -3920,7 +3924,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="141" customFormat="1">
+    <row r="3" spans="1:5" s="142" customFormat="1">
       <c r="A3" s="80" t="s">
         <v>136</v>
       </c>
@@ -3928,7 +3932,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="141" customFormat="1">
+    <row r="4" spans="1:5" s="142" customFormat="1">
       <c r="A4" s="80" t="s">
         <v>138</v>
       </c>
@@ -3936,7 +3940,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="141" customFormat="1">
+    <row r="5" spans="1:5" s="142" customFormat="1">
       <c r="A5" s="80" t="s">
         <v>140</v>
       </c>
@@ -3944,7 +3948,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="141" customFormat="1">
+    <row r="6" spans="1:5" s="142" customFormat="1">
       <c r="A6" s="80" t="s">
         <v>141</v>
       </c>
@@ -3952,7 +3956,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="141" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" s="142" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A7" s="81" t="s">
         <v>143</v>
       </c>
@@ -3967,10 +3971,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="C9" s="82"/>
-      <c r="D9" s="145">
+      <c r="D9" s="146">
         <v>2021</v>
       </c>
-      <c r="E9" s="140"/>
+      <c r="E9" s="141"/>
     </row>
     <row r="10" spans="1:5">
       <c r="C10" s="82"/>
@@ -4103,11 +4107,11 @@
       </c>
     </row>
     <row r="26" spans="3:5">
-      <c r="C26" s="145" t="s">
+      <c r="C26" s="146" t="s">
         <v>324</v>
       </c>
-      <c r="D26" s="140"/>
-      <c r="E26" s="140"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="141"/>
     </row>
     <row r="27" spans="3:5">
       <c r="C27" s="90" t="s">
@@ -4170,20 +4174,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="146" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" style="146" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="147" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="147" customWidth="1"/>
     <col min="3" max="3" width="21.54296875" style="69" customWidth="1"/>
     <col min="4" max="4" width="22.1796875" style="69" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.453125" style="69" customWidth="1"/>
     <col min="7" max="16384" width="11.453125" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="146" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:5" s="147" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="146" customFormat="1">
+    <row r="2" spans="1:5" s="147" customFormat="1">
       <c r="A2" s="79" t="s">
         <v>134</v>
       </c>
@@ -4191,7 +4195,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="146" customFormat="1">
+    <row r="3" spans="1:5" s="147" customFormat="1">
       <c r="A3" s="80" t="s">
         <v>136</v>
       </c>
@@ -4199,7 +4203,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="146" customFormat="1">
+    <row r="4" spans="1:5" s="147" customFormat="1">
       <c r="A4" s="80" t="s">
         <v>138</v>
       </c>
@@ -4207,13 +4211,13 @@
         <v>328</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="146" customFormat="1">
+    <row r="5" spans="1:5" s="147" customFormat="1">
       <c r="A5" s="80" t="s">
         <v>140</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:5" s="146" customFormat="1">
+    <row r="6" spans="1:5" s="147" customFormat="1">
       <c r="A6" s="80" t="s">
         <v>141</v>
       </c>
@@ -4221,7 +4225,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="146" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+    <row r="7" spans="1:5" s="147" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A7" s="81" t="s">
         <v>143</v>
       </c>
@@ -4230,11 +4234,11 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="C8" s="147" t="s">
+      <c r="C8" s="148" t="s">
         <v>331</v>
       </c>
-      <c r="D8" s="148"/>
-      <c r="E8" s="148"/>
+      <c r="D8" s="149"/>
+      <c r="E8" s="149"/>
     </row>
     <row r="9" spans="1:5">
       <c r="C9" s="71"/>
@@ -4308,10 +4312,10 @@
       </c>
     </row>
     <row r="17" spans="3:4">
-      <c r="C17" s="149" t="s">
+      <c r="C17" s="150" t="s">
         <v>336</v>
       </c>
-      <c r="D17" s="148"/>
+      <c r="D17" s="149"/>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="75" t="s">
@@ -4384,7 +4388,7 @@
   <dimension ref="A1:G410"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="E410" sqref="E410"/>
+      <selection activeCell="B410" sqref="B410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -11692,16 +11696,16 @@
       <c r="G409" s="92"/>
     </row>
     <row r="410" spans="1:7">
-      <c r="A410" s="150" t="s">
-        <v>81</v>
-      </c>
-      <c r="B410" s="150" t="s">
+      <c r="A410" s="107" t="s">
         <v>342</v>
       </c>
-      <c r="C410" s="150" t="s">
+      <c r="B410" s="92" t="s">
+        <v>43</v>
+      </c>
+      <c r="C410" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="E410" s="150">
+      <c r="E410" s="107">
         <v>100</v>
       </c>
     </row>
@@ -16291,12 +16295,12 @@
     <col min="1018" max="16384" width="11.453125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:987" s="115" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:987" s="135" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:987" s="115" customFormat="1">
+    <row r="2" spans="1:987" s="135" customFormat="1">
       <c r="A2" s="79" t="s">
         <v>134</v>
       </c>
@@ -16304,7 +16308,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:987" s="115" customFormat="1">
+    <row r="3" spans="1:987" s="135" customFormat="1">
       <c r="A3" s="80" t="s">
         <v>136</v>
       </c>
@@ -16312,7 +16316,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:987" s="115" customFormat="1">
+    <row r="4" spans="1:987" s="135" customFormat="1">
       <c r="A4" s="80" t="s">
         <v>138</v>
       </c>
@@ -16320,7 +16324,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:987" s="115" customFormat="1">
+    <row r="5" spans="1:987" s="135" customFormat="1">
       <c r="A5" s="80" t="s">
         <v>140</v>
       </c>
@@ -16328,7 +16332,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:987" s="115" customFormat="1">
+    <row r="6" spans="1:987" s="135" customFormat="1">
       <c r="A6" s="80" t="s">
         <v>141</v>
       </c>
@@ -16336,7 +16340,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:987" s="115" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+    <row r="7" spans="1:987" s="135" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A7" s="81" t="s">
         <v>143</v>
       </c>
@@ -16345,16 +16349,16 @@
       </c>
     </row>
     <row r="8" spans="1:987" ht="18" customHeight="1">
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="122" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="124"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="124"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -17336,18 +17340,18 @@
       <c r="AKY8" s="7"/>
     </row>
     <row r="9" spans="1:987" ht="25.4" customHeight="1">
-      <c r="C9" s="134" t="s">
+      <c r="C9" s="126" t="s">
         <v>146</v>
       </c>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109"/>
       <c r="M9" s="14"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
@@ -17558,10 +17562,10 @@
       <c r="HJ9" s="13"/>
     </row>
     <row r="10" spans="1:987" ht="17.25" customHeight="1">
-      <c r="C10" s="120"/>
-      <c r="D10" s="121"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="122"/>
+      <c r="C10" s="137"/>
+      <c r="D10" s="138"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="139"/>
       <c r="G10" s="19">
         <v>2015</v>
       </c>
@@ -17585,12 +17589,12 @@
       </c>
       <c r="N10" s="22"/>
       <c r="O10" s="13"/>
-      <c r="P10" s="132"/>
-      <c r="Q10" s="133"/>
-      <c r="R10" s="133"/>
-      <c r="S10" s="133"/>
-      <c r="T10" s="133"/>
-      <c r="U10" s="133"/>
+      <c r="P10" s="123"/>
+      <c r="Q10" s="124"/>
+      <c r="R10" s="124"/>
+      <c r="S10" s="124"/>
+      <c r="T10" s="124"/>
+      <c r="U10" s="124"/>
       <c r="V10" s="23">
         <v>2015</v>
       </c>
@@ -17804,12 +17808,12 @@
       <c r="HJ10" s="13"/>
     </row>
     <row r="11" spans="1:987" ht="14.65" customHeight="1">
-      <c r="C11" s="118" t="s">
+      <c r="C11" s="114" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="109"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="112"/>
       <c r="G11" s="25" t="s">
         <v>149</v>
       </c>
@@ -17835,14 +17839,14 @@
       </c>
       <c r="N11" s="27"/>
       <c r="O11" s="13"/>
-      <c r="P11" s="136" t="s">
+      <c r="P11" s="128" t="s">
         <v>151</v>
       </c>
-      <c r="Q11" s="108"/>
-      <c r="R11" s="108"/>
-      <c r="S11" s="108"/>
-      <c r="T11" s="108"/>
-      <c r="U11" s="109"/>
+      <c r="Q11" s="111"/>
+      <c r="R11" s="111"/>
+      <c r="S11" s="111"/>
+      <c r="T11" s="111"/>
+      <c r="U11" s="112"/>
       <c r="V11" s="28" t="s">
         <v>152</v>
       </c>
@@ -18058,12 +18062,12 @@
       <c r="HJ11" s="13"/>
     </row>
     <row r="12" spans="1:987" ht="14.65" customHeight="1">
-      <c r="C12" s="135" t="s">
+      <c r="C12" s="127" t="s">
         <v>153</v>
       </c>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="109"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="112"/>
       <c r="G12" s="29" t="s">
         <v>154</v>
       </c>
@@ -18091,13 +18095,13 @@
       <c r="N12" s="27"/>
       <c r="O12" s="13"/>
       <c r="P12" s="32"/>
-      <c r="Q12" s="119" t="s">
+      <c r="Q12" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="R12" s="108"/>
-      <c r="S12" s="108"/>
-      <c r="T12" s="108"/>
-      <c r="U12" s="109"/>
+      <c r="R12" s="111"/>
+      <c r="S12" s="111"/>
+      <c r="T12" s="111"/>
+      <c r="U12" s="112"/>
       <c r="V12" s="28" t="s">
         <v>156</v>
       </c>
@@ -18313,12 +18317,12 @@
       <c r="HJ12" s="13"/>
     </row>
     <row r="13" spans="1:987" ht="14.65" customHeight="1">
-      <c r="C13" s="118" t="s">
+      <c r="C13" s="114" t="s">
         <v>157</v>
       </c>
-      <c r="D13" s="108"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="109"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="112"/>
       <c r="G13" s="25" t="s">
         <v>158</v>
       </c>
@@ -18345,13 +18349,13 @@
       <c r="N13" s="27"/>
       <c r="O13" s="33"/>
       <c r="P13" s="34"/>
-      <c r="Q13" s="112" t="s">
+      <c r="Q13" s="110" t="s">
         <v>160</v>
       </c>
-      <c r="R13" s="108"/>
-      <c r="S13" s="108"/>
-      <c r="T13" s="108"/>
-      <c r="U13" s="109"/>
+      <c r="R13" s="111"/>
+      <c r="S13" s="111"/>
+      <c r="T13" s="111"/>
+      <c r="U13" s="112"/>
       <c r="V13" s="35" t="s">
         <v>161</v>
       </c>
@@ -19336,11 +19340,11 @@
     </row>
     <row r="14" spans="1:987" ht="14.65" customHeight="1">
       <c r="C14" s="36"/>
-      <c r="D14" s="111" t="s">
+      <c r="D14" s="133" t="s">
         <v>164</v>
       </c>
-      <c r="E14" s="108"/>
-      <c r="F14" s="109"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="112"/>
       <c r="G14" s="37">
         <v>9839</v>
       </c>
@@ -19365,13 +19369,13 @@
       <c r="N14" s="27"/>
       <c r="O14" s="13"/>
       <c r="P14" s="34"/>
-      <c r="Q14" s="112" t="s">
+      <c r="Q14" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="R14" s="108"/>
-      <c r="S14" s="108"/>
-      <c r="T14" s="108"/>
-      <c r="U14" s="109"/>
+      <c r="R14" s="111"/>
+      <c r="S14" s="111"/>
+      <c r="T14" s="111"/>
+      <c r="U14" s="112"/>
       <c r="V14" s="35" t="s">
         <v>166</v>
       </c>
@@ -19586,11 +19590,11 @@
     </row>
     <row r="15" spans="1:987" ht="14.65" customHeight="1">
       <c r="C15" s="36"/>
-      <c r="D15" s="111" t="s">
+      <c r="D15" s="133" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="108"/>
-      <c r="F15" s="109"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="112"/>
       <c r="G15" s="37">
         <v>1169</v>
       </c>
@@ -19616,12 +19620,12 @@
       <c r="O15" s="13"/>
       <c r="P15" s="32"/>
       <c r="Q15" s="39"/>
-      <c r="R15" s="119" t="s">
+      <c r="R15" s="115" t="s">
         <v>168</v>
       </c>
-      <c r="S15" s="108"/>
-      <c r="T15" s="108"/>
-      <c r="U15" s="109"/>
+      <c r="S15" s="111"/>
+      <c r="T15" s="111"/>
+      <c r="U15" s="112"/>
       <c r="V15" s="28" t="s">
         <v>169</v>
       </c>
@@ -19840,11 +19844,11 @@
     </row>
     <row r="16" spans="1:987" ht="14.65" customHeight="1">
       <c r="C16" s="40"/>
-      <c r="D16" s="110" t="s">
+      <c r="D16" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="108"/>
-      <c r="F16" s="109"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="112"/>
       <c r="G16" s="25">
         <v>5145</v>
       </c>
@@ -19873,11 +19877,11 @@
       <c r="P16" s="32"/>
       <c r="Q16" s="39"/>
       <c r="R16" s="41"/>
-      <c r="S16" s="119" t="s">
+      <c r="S16" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="T16" s="108"/>
-      <c r="U16" s="109"/>
+      <c r="T16" s="111"/>
+      <c r="U16" s="112"/>
       <c r="V16" s="28">
         <v>1275</v>
       </c>
@@ -20865,10 +20869,10 @@
     <row r="17" spans="3:987" ht="14.65" customHeight="1">
       <c r="C17" s="36"/>
       <c r="D17" s="42"/>
-      <c r="E17" s="117" t="s">
+      <c r="E17" s="125" t="s">
         <v>171</v>
       </c>
-      <c r="F17" s="109"/>
+      <c r="F17" s="112"/>
       <c r="G17" s="43">
         <v>2239</v>
       </c>
@@ -20898,11 +20902,11 @@
       <c r="P17" s="34"/>
       <c r="Q17" s="45"/>
       <c r="R17" s="45"/>
-      <c r="S17" s="112" t="s">
+      <c r="S17" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="T17" s="108"/>
-      <c r="U17" s="109"/>
+      <c r="T17" s="111"/>
+      <c r="U17" s="112"/>
       <c r="V17" s="35">
         <v>415</v>
       </c>
@@ -21148,11 +21152,11 @@
       <c r="P18" s="34"/>
       <c r="Q18" s="45"/>
       <c r="R18" s="45"/>
-      <c r="S18" s="112" t="s">
+      <c r="S18" s="110" t="s">
         <v>176</v>
       </c>
-      <c r="T18" s="108"/>
-      <c r="U18" s="109"/>
+      <c r="T18" s="111"/>
+      <c r="U18" s="112"/>
       <c r="V18" s="47"/>
       <c r="W18" s="47"/>
       <c r="X18" s="47"/>
@@ -21391,10 +21395,10 @@
       <c r="Q19" s="45"/>
       <c r="R19" s="45"/>
       <c r="S19" s="45"/>
-      <c r="T19" s="107" t="s">
+      <c r="T19" s="113" t="s">
         <v>171</v>
       </c>
-      <c r="U19" s="109"/>
+      <c r="U19" s="112"/>
       <c r="V19" s="48">
         <v>577</v>
       </c>
@@ -21613,10 +21617,10 @@
     <row r="20" spans="3:987" ht="14.65" customHeight="1">
       <c r="C20" s="36"/>
       <c r="D20" s="42"/>
-      <c r="E20" s="117" t="s">
+      <c r="E20" s="125" t="s">
         <v>179</v>
       </c>
-      <c r="F20" s="109"/>
+      <c r="F20" s="112"/>
       <c r="G20" s="43">
         <v>1109</v>
       </c>
@@ -23135,10 +23139,10 @@
     <row r="23" spans="3:987" ht="14.65" customHeight="1">
       <c r="C23" s="36"/>
       <c r="D23" s="42"/>
-      <c r="E23" s="117" t="s">
+      <c r="E23" s="125" t="s">
         <v>187</v>
       </c>
-      <c r="F23" s="109"/>
+      <c r="F23" s="112"/>
       <c r="G23" s="43">
         <v>87</v>
       </c>
@@ -23167,10 +23171,10 @@
       <c r="Q23" s="45"/>
       <c r="R23" s="45"/>
       <c r="S23" s="45"/>
-      <c r="T23" s="107" t="s">
+      <c r="T23" s="113" t="s">
         <v>179</v>
       </c>
-      <c r="U23" s="109"/>
+      <c r="U23" s="112"/>
       <c r="V23" s="48">
         <v>344</v>
       </c>
@@ -23389,10 +23393,10 @@
     <row r="24" spans="3:987" ht="14.65" customHeight="1">
       <c r="C24" s="36"/>
       <c r="D24" s="42"/>
-      <c r="E24" s="117" t="s">
+      <c r="E24" s="125" t="s">
         <v>188</v>
       </c>
-      <c r="F24" s="109"/>
+      <c r="F24" s="112"/>
       <c r="G24" s="43">
         <v>185</v>
       </c>
@@ -23640,10 +23644,10 @@
     <row r="25" spans="3:987" ht="14.65" customHeight="1">
       <c r="C25" s="36"/>
       <c r="D25" s="42"/>
-      <c r="E25" s="117" t="s">
+      <c r="E25" s="125" t="s">
         <v>190</v>
       </c>
-      <c r="F25" s="109"/>
+      <c r="F25" s="112"/>
       <c r="G25" s="43">
         <v>1263</v>
       </c>
@@ -24174,10 +24178,10 @@
       <c r="Q27" s="45"/>
       <c r="R27" s="45"/>
       <c r="S27" s="45"/>
-      <c r="T27" s="107" t="s">
+      <c r="T27" s="113" t="s">
         <v>187</v>
       </c>
-      <c r="U27" s="109"/>
+      <c r="U27" s="112"/>
       <c r="V27" s="48">
         <v>25</v>
       </c>
@@ -24393,10 +24397,10 @@
     <row r="28" spans="3:987" ht="14.65" customHeight="1">
       <c r="C28" s="36"/>
       <c r="D28" s="42"/>
-      <c r="E28" s="117" t="s">
+      <c r="E28" s="125" t="s">
         <v>195</v>
       </c>
-      <c r="F28" s="109"/>
+      <c r="F28" s="112"/>
       <c r="G28" s="43">
         <v>262</v>
       </c>
@@ -24425,10 +24429,10 @@
       <c r="Q28" s="45"/>
       <c r="R28" s="45"/>
       <c r="S28" s="45"/>
-      <c r="T28" s="107" t="s">
+      <c r="T28" s="113" t="s">
         <v>197</v>
       </c>
-      <c r="U28" s="109"/>
+      <c r="U28" s="112"/>
       <c r="V28" s="48">
         <v>21</v>
       </c>
@@ -24643,11 +24647,11 @@
     </row>
     <row r="29" spans="3:987" ht="14.65" customHeight="1">
       <c r="C29" s="40"/>
-      <c r="D29" s="110" t="s">
+      <c r="D29" s="119" t="s">
         <v>198</v>
       </c>
-      <c r="E29" s="108"/>
-      <c r="F29" s="109"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="112"/>
       <c r="G29" s="25" t="s">
         <v>199</v>
       </c>
@@ -24677,10 +24681,10 @@
       <c r="Q29" s="45"/>
       <c r="R29" s="45"/>
       <c r="S29" s="45"/>
-      <c r="T29" s="107" t="s">
+      <c r="T29" s="113" t="s">
         <v>190</v>
       </c>
-      <c r="U29" s="109"/>
+      <c r="U29" s="112"/>
       <c r="V29" s="48">
         <v>258</v>
       </c>
@@ -25668,20 +25672,20 @@
     <row r="30" spans="3:987">
       <c r="C30" s="36"/>
       <c r="D30" s="42"/>
-      <c r="E30" s="113" t="s">
+      <c r="E30" s="116" t="s">
         <v>200</v>
       </c>
-      <c r="F30" s="109"/>
-      <c r="G30" s="128">
+      <c r="F30" s="112"/>
+      <c r="G30" s="117">
         <v>6348</v>
       </c>
-      <c r="H30" s="128" t="s">
+      <c r="H30" s="117" t="s">
         <v>201</v>
       </c>
-      <c r="I30" s="128">
+      <c r="I30" s="117">
         <v>6494</v>
       </c>
-      <c r="J30" s="128">
+      <c r="J30" s="117">
         <v>6664</v>
       </c>
       <c r="K30" s="31">
@@ -25918,14 +25922,14 @@
     <row r="31" spans="3:987">
       <c r="C31" s="36"/>
       <c r="D31" s="42"/>
-      <c r="E31" s="113" t="s">
+      <c r="E31" s="116" t="s">
         <v>203</v>
       </c>
-      <c r="F31" s="109"/>
-      <c r="G31" s="129"/>
-      <c r="H31" s="129"/>
-      <c r="I31" s="129"/>
-      <c r="J31" s="129"/>
+      <c r="F31" s="112"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="118"/>
+      <c r="I31" s="118"/>
+      <c r="J31" s="118"/>
       <c r="K31" s="31">
         <v>3420.19066666667</v>
       </c>
@@ -26160,10 +26164,10 @@
     <row r="32" spans="3:987">
       <c r="C32" s="36"/>
       <c r="D32" s="42"/>
-      <c r="E32" s="113" t="s">
+      <c r="E32" s="116" t="s">
         <v>205</v>
       </c>
-      <c r="F32" s="109"/>
+      <c r="F32" s="112"/>
       <c r="G32" s="30" t="s">
         <v>206</v>
       </c>
@@ -26191,10 +26195,10 @@
       <c r="Q32" s="45"/>
       <c r="R32" s="45"/>
       <c r="S32" s="45"/>
-      <c r="T32" s="107" t="s">
+      <c r="T32" s="113" t="s">
         <v>195</v>
       </c>
-      <c r="U32" s="109"/>
+      <c r="U32" s="112"/>
       <c r="V32" s="48">
         <v>49</v>
       </c>
@@ -26410,10 +26414,10 @@
     <row r="33" spans="3:987">
       <c r="C33" s="36"/>
       <c r="D33" s="42"/>
-      <c r="E33" s="113" t="s">
+      <c r="E33" s="116" t="s">
         <v>208</v>
       </c>
-      <c r="F33" s="109"/>
+      <c r="F33" s="112"/>
       <c r="G33" s="30">
         <v>90</v>
       </c>
@@ -26441,11 +26445,11 @@
       <c r="P33" s="32"/>
       <c r="Q33" s="39"/>
       <c r="R33" s="39"/>
-      <c r="S33" s="119" t="s">
+      <c r="S33" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="T33" s="108"/>
-      <c r="U33" s="109"/>
+      <c r="T33" s="111"/>
+      <c r="U33" s="112"/>
       <c r="V33" s="28" t="s">
         <v>210</v>
       </c>
@@ -26664,10 +26668,10 @@
     <row r="34" spans="3:987" ht="14.65" customHeight="1">
       <c r="C34" s="36"/>
       <c r="D34" s="42"/>
-      <c r="E34" s="117" t="s">
+      <c r="E34" s="125" t="s">
         <v>211</v>
       </c>
-      <c r="F34" s="109"/>
+      <c r="F34" s="112"/>
       <c r="G34" s="43">
         <v>3734</v>
       </c>
@@ -26696,11 +26700,11 @@
       <c r="P34" s="34"/>
       <c r="Q34" s="45"/>
       <c r="R34" s="45"/>
-      <c r="S34" s="112" t="s">
+      <c r="S34" s="110" t="s">
         <v>212</v>
       </c>
-      <c r="T34" s="108"/>
-      <c r="U34" s="109"/>
+      <c r="T34" s="111"/>
+      <c r="U34" s="112"/>
       <c r="V34" s="35" t="s">
         <v>213</v>
       </c>
@@ -26947,11 +26951,11 @@
       <c r="P35" s="34"/>
       <c r="Q35" s="45"/>
       <c r="R35" s="45"/>
-      <c r="S35" s="112" t="s">
+      <c r="S35" s="110" t="s">
         <v>176</v>
       </c>
-      <c r="T35" s="108"/>
-      <c r="U35" s="109"/>
+      <c r="T35" s="111"/>
+      <c r="U35" s="112"/>
       <c r="V35" s="47"/>
       <c r="W35" s="47"/>
       <c r="X35" s="47"/>
@@ -27190,10 +27194,10 @@
       <c r="Q36" s="45"/>
       <c r="R36" s="45"/>
       <c r="S36" s="45"/>
-      <c r="T36" s="107" t="s">
+      <c r="T36" s="113" t="s">
         <v>217</v>
       </c>
-      <c r="U36" s="109"/>
+      <c r="U36" s="112"/>
       <c r="V36" s="48" t="s">
         <v>218</v>
       </c>
@@ -27412,10 +27416,10 @@
     <row r="37" spans="3:987">
       <c r="C37" s="36"/>
       <c r="D37" s="42"/>
-      <c r="E37" s="113" t="s">
+      <c r="E37" s="116" t="s">
         <v>219</v>
       </c>
-      <c r="F37" s="109"/>
+      <c r="F37" s="112"/>
       <c r="G37" s="30" t="s">
         <v>220</v>
       </c>
@@ -27662,10 +27666,10 @@
     <row r="38" spans="3:987">
       <c r="C38" s="36"/>
       <c r="D38" s="42"/>
-      <c r="E38" s="113" t="s">
+      <c r="E38" s="116" t="s">
         <v>224</v>
       </c>
-      <c r="F38" s="109"/>
+      <c r="F38" s="112"/>
       <c r="G38" s="30">
         <v>531</v>
       </c>
@@ -27910,12 +27914,12 @@
       <c r="HJ38" s="13"/>
     </row>
     <row r="39" spans="3:987" ht="14.65" customHeight="1">
-      <c r="C39" s="118" t="s">
+      <c r="C39" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="108"/>
-      <c r="E39" s="108"/>
-      <c r="F39" s="109"/>
+      <c r="D39" s="111"/>
+      <c r="E39" s="111"/>
+      <c r="F39" s="112"/>
       <c r="G39" s="25" t="s">
         <v>227</v>
       </c>
@@ -27945,10 +27949,10 @@
       <c r="Q39" s="45"/>
       <c r="R39" s="45"/>
       <c r="S39" s="45"/>
-      <c r="T39" s="107" t="s">
+      <c r="T39" s="113" t="s">
         <v>205</v>
       </c>
-      <c r="U39" s="109"/>
+      <c r="U39" s="112"/>
       <c r="V39" s="48" t="s">
         <v>229</v>
       </c>
@@ -28166,11 +28170,11 @@
     </row>
     <row r="40" spans="3:987" ht="14.65" customHeight="1">
       <c r="C40" s="40"/>
-      <c r="D40" s="110" t="s">
+      <c r="D40" s="119" t="s">
         <v>230</v>
       </c>
-      <c r="E40" s="108"/>
-      <c r="F40" s="109"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="112"/>
       <c r="G40" s="25" t="s">
         <v>231</v>
       </c>
@@ -29188,10 +29192,10 @@
     <row r="41" spans="3:987">
       <c r="C41" s="36"/>
       <c r="D41" s="42"/>
-      <c r="E41" s="111" t="s">
+      <c r="E41" s="133" t="s">
         <v>234</v>
       </c>
-      <c r="F41" s="109"/>
+      <c r="F41" s="112"/>
       <c r="G41" s="37">
         <v>5660</v>
       </c>
@@ -29438,10 +29442,10 @@
     <row r="42" spans="3:987" ht="14.65" customHeight="1">
       <c r="C42" s="40"/>
       <c r="D42" s="51"/>
-      <c r="E42" s="110" t="s">
+      <c r="E42" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="109"/>
+      <c r="F42" s="112"/>
       <c r="G42" s="25">
         <v>4442</v>
       </c>
@@ -29469,10 +29473,10 @@
       <c r="Q42" s="45"/>
       <c r="R42" s="45"/>
       <c r="S42" s="45"/>
-      <c r="T42" s="107" t="s">
+      <c r="T42" s="113" t="s">
         <v>208</v>
       </c>
-      <c r="U42" s="109"/>
+      <c r="U42" s="112"/>
       <c r="V42" s="48">
         <v>54</v>
       </c>
@@ -30457,10 +30461,10 @@
     <row r="43" spans="3:987" ht="14.65" customHeight="1">
       <c r="C43" s="40"/>
       <c r="D43" s="51"/>
-      <c r="E43" s="110" t="s">
+      <c r="E43" s="119" t="s">
         <v>198</v>
       </c>
-      <c r="F43" s="109"/>
+      <c r="F43" s="112"/>
       <c r="G43" s="25">
         <v>5677</v>
       </c>
@@ -30491,10 +30495,10 @@
       <c r="Q43" s="45"/>
       <c r="R43" s="45"/>
       <c r="S43" s="45"/>
-      <c r="T43" s="107" t="s">
+      <c r="T43" s="113" t="s">
         <v>211</v>
       </c>
-      <c r="U43" s="109"/>
+      <c r="U43" s="112"/>
       <c r="V43" s="48">
         <v>1341</v>
       </c>
@@ -32233,11 +32237,11 @@
     </row>
     <row r="47" spans="3:987" ht="14.65" customHeight="1">
       <c r="C47" s="40"/>
-      <c r="D47" s="110" t="s">
+      <c r="D47" s="119" t="s">
         <v>244</v>
       </c>
-      <c r="E47" s="108"/>
-      <c r="F47" s="109"/>
+      <c r="E47" s="111"/>
+      <c r="F47" s="112"/>
       <c r="G47" s="25">
         <v>624</v>
       </c>
@@ -33256,10 +33260,10 @@
     <row r="48" spans="3:987" ht="14.65" customHeight="1">
       <c r="C48" s="36"/>
       <c r="D48" s="42"/>
-      <c r="E48" s="111" t="s">
+      <c r="E48" s="133" t="s">
         <v>246</v>
       </c>
-      <c r="F48" s="109"/>
+      <c r="F48" s="112"/>
       <c r="G48" s="37">
         <v>247</v>
       </c>
@@ -33537,10 +33541,10 @@
       <c r="Q49" s="45"/>
       <c r="R49" s="45"/>
       <c r="S49" s="45"/>
-      <c r="T49" s="107" t="s">
+      <c r="T49" s="113" t="s">
         <v>224</v>
       </c>
-      <c r="U49" s="109"/>
+      <c r="U49" s="112"/>
       <c r="V49" s="48">
         <v>240</v>
       </c>
@@ -33785,12 +33789,12 @@
       <c r="O50" s="13"/>
       <c r="P50" s="55"/>
       <c r="Q50" s="56"/>
-      <c r="R50" s="119" t="s">
+      <c r="R50" s="115" t="s">
         <v>249</v>
       </c>
-      <c r="S50" s="108"/>
-      <c r="T50" s="108"/>
-      <c r="U50" s="109"/>
+      <c r="S50" s="111"/>
+      <c r="T50" s="111"/>
+      <c r="U50" s="112"/>
       <c r="V50" s="28">
         <v>31</v>
       </c>
@@ -34004,12 +34008,12 @@
       <c r="HJ50" s="13"/>
     </row>
     <row r="51" spans="3:218" ht="14.65" customHeight="1">
-      <c r="C51" s="118" t="s">
+      <c r="C51" s="114" t="s">
         <v>59</v>
       </c>
-      <c r="D51" s="108"/>
-      <c r="E51" s="108"/>
-      <c r="F51" s="109"/>
+      <c r="D51" s="111"/>
+      <c r="E51" s="111"/>
+      <c r="F51" s="112"/>
       <c r="G51" s="25">
         <v>7642</v>
       </c>
@@ -34036,13 +34040,13 @@
       <c r="N51" s="27"/>
       <c r="O51" s="13"/>
       <c r="P51" s="32"/>
-      <c r="Q51" s="119" t="s">
+      <c r="Q51" s="115" t="s">
         <v>251</v>
       </c>
-      <c r="R51" s="108"/>
-      <c r="S51" s="108"/>
-      <c r="T51" s="108"/>
-      <c r="U51" s="109"/>
+      <c r="R51" s="111"/>
+      <c r="S51" s="111"/>
+      <c r="T51" s="111"/>
+      <c r="U51" s="112"/>
       <c r="V51" s="28">
         <v>220</v>
       </c>
@@ -34260,11 +34264,11 @@
     </row>
     <row r="52" spans="3:218">
       <c r="C52" s="36"/>
-      <c r="D52" s="111" t="s">
+      <c r="D52" s="133" t="s">
         <v>252</v>
       </c>
-      <c r="E52" s="108"/>
-      <c r="F52" s="109"/>
+      <c r="E52" s="111"/>
+      <c r="F52" s="112"/>
       <c r="G52" s="37">
         <v>3411</v>
       </c>
@@ -34290,12 +34294,12 @@
       <c r="O52" s="13"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="45"/>
-      <c r="R52" s="107" t="s">
+      <c r="R52" s="113" t="s">
         <v>253</v>
       </c>
-      <c r="S52" s="108"/>
-      <c r="T52" s="108"/>
-      <c r="U52" s="109"/>
+      <c r="S52" s="111"/>
+      <c r="T52" s="111"/>
+      <c r="U52" s="112"/>
       <c r="V52" s="50">
         <v>144</v>
       </c>
@@ -34510,11 +34514,11 @@
     </row>
     <row r="53" spans="3:218" ht="14.65" customHeight="1">
       <c r="C53" s="36"/>
-      <c r="D53" s="116" t="s">
+      <c r="D53" s="136" t="s">
         <v>254</v>
       </c>
-      <c r="E53" s="108"/>
-      <c r="F53" s="108"/>
+      <c r="E53" s="111"/>
+      <c r="F53" s="111"/>
       <c r="G53" s="43">
         <v>1375</v>
       </c>
@@ -34540,12 +34544,12 @@
       <c r="O53" s="13"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="45"/>
-      <c r="R53" s="107" t="s">
+      <c r="R53" s="113" t="s">
         <v>255</v>
       </c>
-      <c r="S53" s="108"/>
-      <c r="T53" s="108"/>
-      <c r="U53" s="109"/>
+      <c r="S53" s="111"/>
+      <c r="T53" s="111"/>
+      <c r="U53" s="112"/>
       <c r="V53" s="50">
         <v>75</v>
       </c>
@@ -34760,11 +34764,11 @@
     </row>
     <row r="54" spans="3:218" ht="14.65" customHeight="1">
       <c r="C54" s="36"/>
-      <c r="D54" s="125" t="s">
+      <c r="D54" s="130" t="s">
         <v>257</v>
       </c>
-      <c r="E54" s="108"/>
-      <c r="F54" s="109"/>
+      <c r="E54" s="111"/>
+      <c r="F54" s="112"/>
       <c r="G54" s="43">
         <v>3391</v>
       </c>
@@ -34788,17 +34792,17 @@
       </c>
       <c r="N54" s="27"/>
       <c r="O54" s="13"/>
-      <c r="P54" s="138"/>
-      <c r="Q54" s="127"/>
-      <c r="R54" s="127"/>
-      <c r="S54" s="127"/>
-      <c r="T54" s="127"/>
-      <c r="U54" s="127"/>
-      <c r="V54" s="127"/>
-      <c r="W54" s="127"/>
-      <c r="X54" s="127"/>
-      <c r="Y54" s="127"/>
-      <c r="Z54" s="127"/>
+      <c r="P54" s="120"/>
+      <c r="Q54" s="121"/>
+      <c r="R54" s="121"/>
+      <c r="S54" s="121"/>
+      <c r="T54" s="121"/>
+      <c r="U54" s="121"/>
+      <c r="V54" s="121"/>
+      <c r="W54" s="121"/>
+      <c r="X54" s="121"/>
+      <c r="Y54" s="121"/>
+      <c r="Z54" s="121"/>
       <c r="AA54" s="57"/>
       <c r="AB54" s="57"/>
       <c r="AC54" s="13"/>
@@ -34994,11 +34998,11 @@
     </row>
     <row r="55" spans="3:218" ht="14.65" customHeight="1">
       <c r="C55" s="36"/>
-      <c r="D55" s="125" t="s">
+      <c r="D55" s="130" t="s">
         <v>258</v>
       </c>
-      <c r="E55" s="108"/>
-      <c r="F55" s="109"/>
+      <c r="E55" s="111"/>
+      <c r="F55" s="112"/>
       <c r="G55" s="43" t="s">
         <v>259</v>
       </c>
@@ -35229,14 +35233,14 @@
       <c r="HJ55" s="13"/>
     </row>
     <row r="56" spans="3:218" ht="6.25" customHeight="1">
-      <c r="C56" s="126"/>
-      <c r="D56" s="126"/>
-      <c r="E56" s="126"/>
-      <c r="F56" s="127"/>
-      <c r="G56" s="127"/>
-      <c r="H56" s="127"/>
-      <c r="I56" s="127"/>
-      <c r="J56" s="127"/>
+      <c r="C56" s="131"/>
+      <c r="D56" s="131"/>
+      <c r="E56" s="131"/>
+      <c r="F56" s="121"/>
+      <c r="G56" s="121"/>
+      <c r="H56" s="121"/>
+      <c r="I56" s="121"/>
+      <c r="J56" s="121"/>
       <c r="K56" s="59"/>
       <c r="L56" s="60"/>
       <c r="M56" s="60"/>
@@ -35449,16 +35453,16 @@
       <c r="HJ56" s="13"/>
     </row>
     <row r="57" spans="3:218" ht="14.25" customHeight="1">
-      <c r="C57" s="137" t="s">
+      <c r="C57" s="108" t="s">
         <v>262</v>
       </c>
-      <c r="D57" s="124"/>
-      <c r="E57" s="124"/>
-      <c r="F57" s="124"/>
-      <c r="G57" s="124"/>
-      <c r="H57" s="124"/>
-      <c r="I57" s="124"/>
-      <c r="J57" s="124"/>
+      <c r="D57" s="109"/>
+      <c r="E57" s="109"/>
+      <c r="F57" s="109"/>
+      <c r="G57" s="109"/>
+      <c r="H57" s="109"/>
+      <c r="I57" s="109"/>
+      <c r="J57" s="109"/>
       <c r="K57" s="59"/>
       <c r="L57" s="60"/>
       <c r="M57" s="60"/>
@@ -35686,29 +35690,29 @@
       <c r="AB58" s="15"/>
     </row>
     <row r="59" spans="3:218" ht="11.5" customHeight="1">
-      <c r="C59" s="130" t="s">
+      <c r="C59" s="132" t="s">
         <v>264</v>
       </c>
-      <c r="D59" s="124"/>
-      <c r="E59" s="124"/>
-      <c r="F59" s="124"/>
-      <c r="G59" s="124"/>
-      <c r="H59" s="124"/>
-      <c r="I59" s="124"/>
-      <c r="J59" s="124"/>
+      <c r="D59" s="109"/>
+      <c r="E59" s="109"/>
+      <c r="F59" s="109"/>
+      <c r="G59" s="109"/>
+      <c r="H59" s="109"/>
+      <c r="I59" s="109"/>
+      <c r="J59" s="109"/>
       <c r="K59" s="63"/>
       <c r="L59" s="64"/>
       <c r="M59" s="64"/>
-      <c r="P59" s="123" t="s">
+      <c r="P59" s="129" t="s">
         <v>264</v>
       </c>
-      <c r="Q59" s="124"/>
-      <c r="R59" s="124"/>
-      <c r="S59" s="124"/>
-      <c r="T59" s="124"/>
-      <c r="U59" s="124"/>
-      <c r="V59" s="124"/>
-      <c r="W59" s="124"/>
+      <c r="Q59" s="109"/>
+      <c r="R59" s="109"/>
+      <c r="S59" s="109"/>
+      <c r="T59" s="109"/>
+      <c r="U59" s="109"/>
+      <c r="V59" s="109"/>
+      <c r="W59" s="109"/>
       <c r="X59" s="57"/>
       <c r="Y59" s="57"/>
       <c r="Z59" s="57"/>
@@ -35717,6 +35721,63 @@
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="R53:U53"/>
+    <mergeCell ref="T49:U49"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="S34:U34"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="R52:U52"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="C1:XFD7"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="P59:W59"/>
+    <mergeCell ref="Q51:U51"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="S35:U35"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="C56:J56"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="C59:J59"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="T43:U43"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="P10:U10"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="Q12:U12"/>
+    <mergeCell ref="P11:U11"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="C57:J57"/>
     <mergeCell ref="S17:U17"/>
     <mergeCell ref="T27:U27"/>
@@ -35733,63 +35794,6 @@
     <mergeCell ref="I30:I31"/>
     <mergeCell ref="P54:Z54"/>
     <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="P10:U10"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="Q12:U12"/>
-    <mergeCell ref="P11:U11"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="P59:W59"/>
-    <mergeCell ref="Q51:U51"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="S35:U35"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="C56:J56"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="C59:J59"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="T43:U43"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="C1:XFD7"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="R15:U15"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="R53:U53"/>
-    <mergeCell ref="T49:U49"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="S34:U34"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="R52:U52"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="T36:U36"/>
   </mergeCells>
   <pageMargins left="0.47283464566929129" right="0.41456692913385818" top="0.71259842519685035" bottom="0.73937007874015737" header="0.31889763779527558" footer="0.34566929133858271"/>
   <pageSetup paperSize="0" pageOrder="overThenDown" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -35800,6 +35804,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010054A0A362C8B81F47807DE03BF445B4E9" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2af24296270ba5d162585d35a02b2378">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="253d9861-5057-4c6b-aa55-c1bece854d8d" xmlns:ns3="21da35c6-efe3-499f-bfdd-69ff62f566e5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7094bbdd7f50806a56362c1dd47d9fc8" ns2:_="" ns3:_="">
     <xsd:import namespace="253d9861-5057-4c6b-aa55-c1bece854d8d"/>
@@ -36028,16 +36041,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55F570A8-ABD2-4C3A-9929-D441E02FFADE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D097E46-0647-47DB-85A8-2CE500405CD9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36056,14 +36068,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55F570A8-ABD2-4C3A-9929-D441E02FFADE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{219619fd-75dc-48cb-820d-8f683a95dd8b}" enabled="1" method="Privileged" siteId="{05c95b33-90ca-49d5-b644-288b930b912b}" removed="0"/>

</xml_diff>